<commit_message>
update TA with new stock selection code  by main.ipynb
</commit_message>
<xml_diff>
--- a/a_stock_codes_by_concept.xlsx
+++ b/a_stock_codes_by_concept.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AI智能体" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ERP概念" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="eSIM" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="低碳冶金" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="供销社概念" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="光伏高速公路" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="可燃冰" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="粮食概念" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="转基因" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="乳业" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="免税概念" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="冰雪经济" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="新零售" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="昨日连板" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="昨日连板_含一字" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="社区团购" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="退税商店" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="预制菜概念" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="鸡肉概念" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,240 +457,372 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>002315</t>
+          <t>001219</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>焦点科技</t>
+          <t>青岛食品</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>002530</t>
+          <t>001318</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>金财互联</t>
+          <t>阳光乳业</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002657</t>
+          <t>002329</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>中科金财</t>
+          <t>皇氏集团</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002757</t>
+          <t>002385</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>南兴股份</t>
+          <t>大北农</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>300010</t>
+          <t>002458</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>豆神教育</t>
+          <t>益生股份</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>300130</t>
+          <t>002557</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>新国都</t>
+          <t>洽洽食品</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>300170</t>
+          <t>002570</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>汉得信息</t>
+          <t>贝因美</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300248</t>
+          <t>002719</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>新开普</t>
+          <t>麦趣尔</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>300378</t>
+          <t>002732</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>鼎捷数智</t>
+          <t>燕塘乳业</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>300384</t>
+          <t>002910</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>三联虹普</t>
+          <t>庄园牧场</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>300479</t>
+          <t>002946</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>神思电子</t>
+          <t>新乳业</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>300608</t>
+          <t>300106</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>思特奇</t>
+          <t>西部牧业</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>300624</t>
+          <t>300498</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>万兴科技</t>
+          <t>温氏股份</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>300634</t>
+          <t>300858</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>彩讯股份</t>
+          <t>科拓生物</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>300654</t>
+          <t>300892</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>世纪天鸿</t>
+          <t>品渥食品</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>300840</t>
+          <t>300898</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>酷特智能</t>
+          <t>熊猫乳品</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>300996</t>
+          <t>300915</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>普联软件</t>
+          <t>海融科技</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>301396</t>
+          <t>600127</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>宏景科技</t>
+          <t>金健米业</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>601360</t>
+          <t>600300</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>三六零</t>
+          <t>维维股份</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>688132</t>
+          <t>600419</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>邦彦技术</t>
+          <t>天润乳业</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>600429</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>三元股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>600597</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>光明乳业</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>600882</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>妙可蓝多</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>600887</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>伊利股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>600965</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>福成股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>605179</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>一鸣食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>605337</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>李子园</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>605339</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>南侨食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>605388</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>均瑶健康</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>688089</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>嘉必优</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>832786</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>骑士乳业</t>
         </is>
       </c>
     </row>
@@ -976,7 +1108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,204 +1131,324 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>002232</t>
+          <t>000501</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>启明信息</t>
+          <t>武商集团</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>002315</t>
+          <t>000524</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>焦点科技</t>
+          <t>岭南控股</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002398</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>垒知集团</t>
+          <t>供销大集</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>300131</t>
+          <t>000759</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>英唐智控</t>
+          <t>中百集团</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>300170</t>
+          <t>000796</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>汉得信息</t>
+          <t>凯撒旅业</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>300195</t>
+          <t>000886</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>长荣股份</t>
+          <t>海南高速</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>300378</t>
+          <t>001979</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>鼎捷数智</t>
+          <t>招商蛇口</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300668</t>
+          <t>002163</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>杰恩设计</t>
+          <t>海南发展</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>300687</t>
+          <t>002251</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>赛意信息</t>
+          <t>步步高</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>300807</t>
+          <t>002277</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>天迈科技</t>
+          <t>友阿股份</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>300996</t>
+          <t>002707</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>普联软件</t>
+          <t>众信旅游</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>301315</t>
+          <t>600009</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>威士顿</t>
+          <t>上海机场</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>600588</t>
+          <t>600018</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>用友网络</t>
+          <t>上港集团</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>600845</t>
+          <t>600029</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>宝信软件</t>
+          <t>南方航空</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>688365</t>
+          <t>600185</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>光云科技</t>
+          <t>珠免集团</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>688369</t>
+          <t>600415</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>致远互联</t>
+          <t>小商品城</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>688631</t>
+          <t>600515</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>莱斯信息</t>
+          <t>海南机场</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>600693</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>东百集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>600694</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>大商股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>600697</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>欧亚集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>600712</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>南宁百货</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>600827</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>百联股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>600859</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>王府井</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>601021</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>春秋航空</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>601118</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>海南橡胶</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>601888</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>中国中免</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>603069</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>海汽集团</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1234,120 +1486,432 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>002017</t>
+          <t>000069</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>东信和平</t>
+          <t>华侨城Ａ</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>002049</t>
+          <t>000501</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>紫光国微</t>
+          <t>武商集团</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002104</t>
+          <t>000530</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>恒宝股份</t>
+          <t>冰山冷热</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002881</t>
+          <t>000558</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>美格智能</t>
+          <t>天府文旅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>003040</t>
+          <t>000811</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>楚天龙</t>
+          <t>冰轮环境</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>300002</t>
+          <t>000888</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>神州泰岳</t>
+          <t>峨眉山Ａ</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>300205</t>
+          <t>001368</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ST天喻</t>
+          <t>通达创智</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300638</t>
+          <t>002033</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>广和通</t>
+          <t>丽江股份</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>300689</t>
+          <t>002051</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>澄天伟业</t>
+          <t>中工国际</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>600050</t>
+          <t>002159</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>中国联通</t>
+          <t>三特索道</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>002354</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>天娱数科</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>002523</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>天桥起重</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>002639</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>雪人集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>002659</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>凯文教育</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>002701</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>奥瑞金</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>002780</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>三夫户外</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>002887</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>绿茵生态</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>002899</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>英派斯</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>300005</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>探路者</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>300133</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>华策影视</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>300859</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>西域旅游</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>300860</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>锋尚文化</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>301010</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>晶雪节能</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>301058</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>中粮科工</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>301187</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>欧圣电气</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>301287</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>康力源</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>600138</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>中青旅</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>600158</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>中体产业</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>600325</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>华发股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>600593</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>大连圣亚</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>600628</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>新世界</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>600697</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>欧亚集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>600749</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>西藏旅游</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>600853</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>龙建股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>600859</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>王府井</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>603099</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>长白山</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1385,96 +1949,1740 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000709</t>
+          <t>000017</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>河钢股份</t>
+          <t>深中华A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000928</t>
+          <t>000061</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>中钢国际</t>
+          <t>农 产 品</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000959</t>
+          <t>000417</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>首钢股份</t>
+          <t>合百集团</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>600019</t>
+          <t>000419</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>宝钢股份</t>
+          <t>通程控股</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>600307</t>
+          <t>000501</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>酒钢宏兴</t>
+          <t>武商集团</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>600388</t>
+          <t>000505</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>龙净环保</t>
+          <t>京粮控股</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>600581</t>
+          <t>000523</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>八一钢铁</t>
+          <t>红棉股份</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>601618</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>中国中冶</t>
+          <t>供销大集</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>000639</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>西王食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>000651</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>格力电器</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>000679</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>大连友谊</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>000681</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>视觉中国</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>000725</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>京东方Ａ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>000726</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>鲁  泰Ａ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>000756</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>新华制药</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>000759</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>中百集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>000785</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>居然智家</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>000848</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>承德露露</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>000858</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>五 粮 液</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>000882</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>华联股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>000895</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>双汇发展</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>001219</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>青岛食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>001222</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>源飞宠物</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>002024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ST易购</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>002035</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>华帝股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>002094</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>青岛金王</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>002127</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>南极电商</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>002153</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>石基信息</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>002183</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>怡 亚 通</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>002186</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>全 聚 德</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>002187</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>广百股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>002193</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>如意集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>002251</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>002264</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>新 华 都</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>002269</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>美邦服饰</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>002277</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>友阿股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>002293</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>罗莱生活</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>002321</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>华英农业</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>002345</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>潮宏基</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>002376</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>新北洋</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>002397</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>梦洁股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>002416</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>爱施德</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>002419</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>天虹股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>002488</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>金固股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>002515</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>金字火腿</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>002561</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>徐家汇</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>002563</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>森马服饰</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>002566</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>益盛药业</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>002572</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>索菲亚</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>002612</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>朗姿股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>002614</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>奥佳华</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>002615</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>哈尔斯</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>002650</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ST加加</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>002678</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>珠江钢琴</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>002697</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>红旗连锁</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>002702</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>海欣食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>002719</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>麦趣尔</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>002726</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>龙大美食</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>002762</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>*ST金比</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>002780</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>三夫户外</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>002820</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>桂发祥</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>002832</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>比音勒芬</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>002875</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>安奈儿</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>002946</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>新乳业</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>002991</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>甘源食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>003012</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>东鹏控股</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>003016</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>欣贺股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>003030</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>祖名股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>300094</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>国联水产</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>300162</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>雷曼光电</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>300268</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>*ST佳沃</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>300378</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>鼎捷数智</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>300441</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>鲍斯股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>300498</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>温氏股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>300755</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>华致酒行</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>300892</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>品渥食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>300908</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>仲景食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>300945</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>曼卡龙</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>300972</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>万辰集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>600127</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>金健米业</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>600185</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>珠免集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>600186</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>莲花控股</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>600280</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>中央商场</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>600327</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>大东方</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>600335</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>国机汽车</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>600336</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>澳柯玛</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>600398</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>海澜之家</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>600400</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>红豆股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>600439</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>瑞贝卡</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>600597</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>光明乳业</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>600600</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>青岛啤酒</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>600628</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>新世界</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>600630</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>龙头股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>600655</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>豫园股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>600697</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>欧亚集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>600702</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>舍得酒业</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>600712</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>南宁百货</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>600738</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>丽尚国潮</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>600771</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>广誉远</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>600774</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>汉商集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>600778</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>友好集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>600785</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>新华百货</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>600814</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>杭州解百</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>600824</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>益民集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>600827</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>百联股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>600838</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>上海九百</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>600858</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>银座股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>600859</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>王府井</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>600882</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>妙可蓝多</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>600887</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>伊利股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>600983</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>惠而浦</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>601086</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>国芳集团</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>601116</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>三江购物</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>601366</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>利群股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>601566</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>九牧王</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>601801</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>皖新传媒</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>601828</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>美凯龙</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>601933</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>永辉超市</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>603001</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>奥康国际</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>603008</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>喜临门</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>603031</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>安孚科技</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>603101</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>汇嘉时代</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>603116</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>红蜻蜓</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>603123</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>翠微股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>603193</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>润本股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>603214</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>爱婴室</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>603336</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>宏辉果蔬</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>603517</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>绝味食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>603536</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>惠发食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>603557</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>ST起步</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>603608</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>天创时尚</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>603630</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>拉芳家化</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>603668</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>天马科技</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>603708</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>家家悦</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>603719</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>良品铺子</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>603777</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>来伊份</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>603825</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>ST华扬</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>603877</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>太平鸟</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>603900</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>莱绅通灵</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>605136</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>丽人丽妆</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>605188</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>国光连锁</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>605499</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>东鹏饮料</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>605567</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>春雪食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>688365</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>光云科技</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>838262</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>太湖雪</t>
         </is>
       </c>
     </row>
@@ -1489,7 +3697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1512,168 +3720,60 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000564</t>
+          <t>002021</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>供销大集</t>
+          <t>中捷资源</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000722</t>
+          <t>300092</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>湖南发展</t>
+          <t>科新机电</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000893</t>
+          <t>601069</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>亚钾国际</t>
+          <t>西部黄金</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002014</t>
+          <t>603051</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>永新股份</t>
+          <t>鹿山新材</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>002556</t>
+          <t>837174</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>辉隆股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>002643</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>万润股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>002758</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>浙农股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>002999</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>天禾股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>003042</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>中农联合</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>600217</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>中再资环</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>600318</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>新力金融</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>600354</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>敦煌种业</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>603029</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>天鹅股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>603970</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>中农立华</t>
+          <t>宏裕包材</t>
         </is>
       </c>
     </row>
@@ -1688,7 +3788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1711,84 +3811,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000755</t>
+          <t>002021</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>山西高速</t>
+          <t>中捷资源</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000900</t>
+          <t>002547</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>现代投资</t>
+          <t>春兴精工</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>300365</t>
+          <t>002975</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>恒华科技</t>
+          <t>博杰股份</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>600035</t>
+          <t>300092</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>楚天高速</t>
+          <t>科新机电</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>600098</t>
+          <t>601069</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>广州发展</t>
+          <t>西部黄金</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>600269</t>
+          <t>603051</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>赣粤高速</t>
+          <t>鹿山新材</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>600350</t>
+          <t>603839</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>山东高速</t>
+          <t>安正时尚</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>605255</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>天普股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>837174</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>宏裕包材</t>
         </is>
       </c>
     </row>
@@ -1803,7 +3927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1826,180 +3950,444 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000039</t>
+          <t>000501</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>中集集团</t>
+          <t>武商集团</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000852</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>石化机械</t>
+          <t>供销大集</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002207</t>
+          <t>000607</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>准油股份</t>
+          <t>华媒控股</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002278</t>
+          <t>000610</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>神开股份</t>
+          <t>西安旅游</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>002353</t>
+          <t>000721</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>杰瑞股份</t>
+          <t>西安饮食</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002554</t>
+          <t>000759</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>惠博普</t>
+          <t>中百集团</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>300084</t>
+          <t>000895</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>海默科技</t>
+          <t>双汇发展</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300191</t>
+          <t>002251</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>潜能恒信</t>
+          <t>步步高</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>600098</t>
+          <t>002299</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>广州发展</t>
+          <t>圣农发展</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>600282</t>
+          <t>002494</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>南钢股份</t>
+          <t>华斯股份</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>600583</t>
+          <t>002561</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>海油工程</t>
+          <t>徐家汇</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>600871</t>
+          <t>002563</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>石化油服</t>
+          <t>森马服饰</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>601808</t>
+          <t>002650</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>中海油服</t>
+          <t>ST加加</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>603699</t>
+          <t>002695</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>纽威股份</t>
+          <t>煌上煌</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>603727</t>
+          <t>002702</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>博迈科</t>
+          <t>海欣食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>002726</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>龙大美食</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>002991</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>甘源食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>003000</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>劲仔食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>003010</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>若羽臣</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>003030</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>祖名股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>300094</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>国联水产</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>300892</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>品渥食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>300908</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>仲景食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>300999</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>金龙鱼</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>600113</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>浙江东日</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>600327</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>大东方</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>600779</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>水井坊</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>600882</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>妙可蓝多</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>601116</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>三江购物</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>601366</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>利群股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>601933</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>永辉超市</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>603336</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>宏辉果蔬</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>603506</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>南都物业</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>603536</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>惠发食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>603708</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>家家悦</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>603719</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>良品铺子</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>603777</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>来伊份</t>
         </is>
       </c>
     </row>
@@ -2014,7 +4402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2037,348 +4425,144 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000019</t>
+          <t>000417</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>深粮控股</t>
+          <t>合百集团</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000638</t>
+          <t>002187</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>万方发展</t>
+          <t>广百股份</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000713</t>
+          <t>002404</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>丰乐种业</t>
+          <t>嘉欣丝绸</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000716</t>
+          <t>600415</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>黑芝麻</t>
+          <t>小商品城</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000998</t>
+          <t>600628</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>隆平高科</t>
+          <t>新世界</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002041</t>
+          <t>600655</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>登海种业</t>
+          <t>豫园股份</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>002133</t>
+          <t>600712</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>广宇集团</t>
+          <t>南宁百货</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>002385</t>
+          <t>600814</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>大北农</t>
+          <t>杭州解百</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>002419</t>
+          <t>600827</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>天虹股份</t>
+          <t>百联股份</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>002646</t>
+          <t>600828</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>天佑德酒</t>
+          <t>茂业商业</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>002758</t>
+          <t>600865</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>浙农股份</t>
+          <t>百大集团</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>002999</t>
+          <t>603123</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>天禾股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>300087</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>荃银高科</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>300189</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>神农种业</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>600108</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>亚盛集团</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>600127</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>金健米业</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>600191</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>华资实业</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>600300</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>维维股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>600313</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>农发种业</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>600354</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>敦煌种业</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>600359</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>新农开发</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>600540</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>新赛股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>600598</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>北大荒</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>600704</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>物产中大</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>600811</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>东方集团</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>601952</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>苏垦农发</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>603182</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>嘉华股份</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>430476</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>海能技术</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>837403</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>康农种业</t>
+          <t>翠微股份</t>
         </is>
       </c>
     </row>
@@ -2393,7 +4577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2416,192 +4600,696 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000713</t>
+          <t>000019</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>丰乐种业</t>
+          <t>深粮控股</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000998</t>
+          <t>000417</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>隆平高科</t>
+          <t>合百集团</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002041</t>
+          <t>000428</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>登海种业</t>
+          <t>华天酒店</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002100</t>
+          <t>000524</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>天康生物</t>
+          <t>岭南控股</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>002170</t>
+          <t>000529</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>芭田股份</t>
+          <t>广弘控股</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002385</t>
+          <t>000564</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>大北农</t>
+          <t>供销大集</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>300087</t>
+          <t>000721</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>荃银高科</t>
+          <t>西安饮食</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300197</t>
+          <t>000895</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>节能铁汉</t>
+          <t>双汇发展</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>301556</t>
+          <t>001211</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>托普云农</t>
+          <t>双枪科技</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>600313</t>
+          <t>001215</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>农发种业</t>
+          <t>千味央厨</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>600354</t>
+          <t>001313</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>敦煌种业</t>
+          <t>粤海饲料</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>600371</t>
+          <t>002069</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>万向德农</t>
+          <t>獐子岛</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>600596</t>
+          <t>002086</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>新安股份</t>
+          <t>东方海洋</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>688265</t>
+          <t>002100</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>南模生物</t>
+          <t>天康生物</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>833819</t>
+          <t>002124</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>颖泰生物</t>
+          <t>天邦食品</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>837403</t>
+          <t>002186</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>康农种业</t>
+          <t>全 聚 德</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>002187</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>广百股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>002216</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>三全食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>002251</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>步步高</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>002299</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>圣农发展</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>002321</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>华英农业</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>002330</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>得利斯</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>002481</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>双塔食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>002515</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>金字火腿</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>002567</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>唐人神</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>002661</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>克明食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>002696</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>百洋股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>002701</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>奥瑞金</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>002702</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>海欣食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>002726</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>龙大美食</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>002746</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>仙坛股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>002820</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>桂发祥</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>002982</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>湘佳股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>300094</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>国联水产</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>300501</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>海顺新材</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>300999</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>金龙鱼</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>301116</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>益客食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>600073</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>光明肉业</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>600127</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>金健米业</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>600257</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>大湖股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>600467</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>好当家</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>600883</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>博闻科技</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>600965</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>福成股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>601007</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>金陵饭店</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>601366</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>利群股份</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>601933</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>永辉超市</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>603043</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>广州酒家</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>603057</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>紫燕食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>603237</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>五芳斋</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>603345</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>安井食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>603536</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>惠发食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>605089</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>味知香</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>605108</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>同庆楼</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>605136</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>丽人丽妆</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>605567</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>春雪食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>430476</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>海能技术</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>836826</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>盖世食品</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>839273</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>一致魔芋</t>
         </is>
       </c>
     </row>

</xml_diff>